<commit_message>
all calculations ready, now route names, schemes and bus type coloring
</commit_message>
<xml_diff>
--- a/downloads/asdasd.xlsx
+++ b/downloads/asdasd.xlsx
@@ -96,11 +96,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode=""/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="[mm]:ss"/>
-    <numFmt numFmtId="167" formatCode="[hh]:mm"/>
+    <numFmt numFmtId="165" formatCode="[mm]:ss"/>
+    <numFmt numFmtId="166" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -279,13 +278,13 @@
     <xf numFmtId="1" fontId="9" fillId="11" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="11" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="11" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+    <xf numFmtId="165" fontId="11" fillId="11" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -515,6 +514,13 @@
       <c r="J5" t="n" s="10">
         <v>71.0</v>
       </c>
+      <c r="K5" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5" t="n" s="12">
+        <v>0.9770833333333333</v>
+      </c>
       <c r="O5" t="n" s="12">
         <v>0.925</v>
       </c>
@@ -553,6 +559,13 @@
       <c r="J6" t="n" s="10">
         <v>92.0</v>
       </c>
+      <c r="K6" t="n" s="12">
+        <v>0.28125</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6" t="n" s="12">
+        <v>0.9826388888888888</v>
+      </c>
       <c r="O6" t="n" s="12">
         <v>0.9340277777777778</v>
       </c>
@@ -589,7 +602,14 @@
         <v>0.06666666666666667</v>
       </c>
       <c r="J7" t="n" s="10">
-        <v>55.0</v>
+        <v>55.5</v>
+      </c>
+      <c r="K7" t="n" s="12">
+        <v>0.2847222222222222</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7" t="n" s="12">
+        <v>0.9736111111111111</v>
       </c>
       <c r="O7" t="n" s="12">
         <v>0.9180555555555555</v>
@@ -627,7 +647,14 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="J8" t="n" s="10">
-        <v>22.0</v>
+        <v>22.5</v>
+      </c>
+      <c r="K8" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8" t="n" s="12">
+        <v>0.9840277777777777</v>
       </c>
       <c r="O8" t="n" s="12">
         <v>0.9145833333333333</v>
@@ -667,6 +694,13 @@
       <c r="J9" t="n" s="10">
         <v>14.0</v>
       </c>
+      <c r="K9" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9" t="n" s="12">
+        <v>0.9583333333333334</v>
+      </c>
       <c r="O9" t="n" s="12">
         <v>0.875</v>
       </c>
@@ -703,7 +737,14 @@
         <v>0.09722222222222222</v>
       </c>
       <c r="J10" t="n" s="10">
-        <v>44.0</v>
+        <v>44.5</v>
+      </c>
+      <c r="K10" t="n" s="12">
+        <v>0.3055555555555556</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10" t="n" s="12">
+        <v>1.0</v>
       </c>
       <c r="O10" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -741,7 +782,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J11" t="n" s="10">
-        <v>44.0</v>
+        <v>44.5</v>
+      </c>
+      <c r="K11" t="n" s="12">
+        <v>0.2847222222222222</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11" t="n" s="12">
+        <v>0.9722222222222222</v>
       </c>
       <c r="O11" t="n" s="12">
         <v>0.9375</v>
@@ -781,6 +829,13 @@
       <c r="J12" t="n" s="10">
         <v>62.0</v>
       </c>
+      <c r="K12" t="n" s="12">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12" t="n" s="12">
+        <v>0.9736111111111111</v>
+      </c>
       <c r="O12" t="n" s="12">
         <v>0.9215277777777777</v>
       </c>
@@ -817,7 +872,14 @@
         <v>0.10694444444444444</v>
       </c>
       <c r="J13" t="n" s="10">
-        <v>23.0</v>
+        <v>23.5</v>
+      </c>
+      <c r="K13" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L13"/>
+      <c r="M13" t="n" s="12">
+        <v>0.9902777777777778</v>
       </c>
       <c r="O13" t="n" s="12">
         <v>0.9097222222222222</v>
@@ -857,6 +919,13 @@
       <c r="J14" t="n" s="10">
         <v>49.0</v>
       </c>
+      <c r="K14" t="n" s="12">
+        <v>0.2861111111111111</v>
+      </c>
+      <c r="L14"/>
+      <c r="M14" t="n" s="12">
+        <v>0.9923611111111111</v>
+      </c>
       <c r="O14" t="n" s="12">
         <v>0.9236111111111112</v>
       </c>
@@ -895,6 +964,13 @@
       <c r="J15" t="n" s="10">
         <v>34.0</v>
       </c>
+      <c r="K15" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L15"/>
+      <c r="M15" t="n" s="12">
+        <v>0.9909722222222223</v>
+      </c>
       <c r="O15" t="n" s="12">
         <v>0.8986111111111111</v>
       </c>
@@ -931,7 +1007,14 @@
         <v>0.09930555555555555</v>
       </c>
       <c r="J16" t="n" s="10">
-        <v>67.0</v>
+        <v>67.5</v>
+      </c>
+      <c r="K16" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L16"/>
+      <c r="M16" t="n" s="12">
+        <v>0.9958333333333333</v>
       </c>
       <c r="O16" t="n" s="12">
         <v>0.9055555555555556</v>
@@ -969,7 +1052,14 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="J17" t="n" s="10">
-        <v>43.0</v>
+        <v>43.5</v>
+      </c>
+      <c r="K17" t="n" s="12">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="L17"/>
+      <c r="M17" t="n" s="12">
+        <v>0.9791666666666666</v>
       </c>
       <c r="O17" t="n" s="12">
         <v>0.9097222222222222</v>
@@ -1007,7 +1097,14 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="J18" t="n" s="10">
-        <v>6.0</v>
+        <v>6.5</v>
+      </c>
+      <c r="K18" t="n" s="12">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="L18"/>
+      <c r="M18" t="n" s="12">
+        <v>0.9166666666666666</v>
       </c>
       <c r="O18" t="n" s="12">
         <v>0.8125</v>
@@ -1047,6 +1144,13 @@
       <c r="J19" t="n" s="10">
         <v>58.0</v>
       </c>
+      <c r="K19" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L19"/>
+      <c r="M19" t="n" s="12">
+        <v>0.9791666666666666</v>
+      </c>
       <c r="O19" t="n" s="12">
         <v>0.90625</v>
       </c>
@@ -1085,6 +1189,13 @@
       <c r="J20" t="n" s="10">
         <v>23.0</v>
       </c>
+      <c r="K20" t="n" s="12">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="L20"/>
+      <c r="M20" t="n" s="12">
+        <v>0.9861111111111112</v>
+      </c>
       <c r="O20" t="n" s="12">
         <v>0.9027777777777778</v>
       </c>
@@ -1121,7 +1232,14 @@
         <v>0.0763888888888889</v>
       </c>
       <c r="J21" t="n" s="10">
-        <v>82.0</v>
+        <v>82.5</v>
+      </c>
+      <c r="K21" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L21"/>
+      <c r="M21" t="n" s="12">
+        <v>0.9868055555555556</v>
       </c>
       <c r="O21" t="n" s="12">
         <v>0.9333333333333333</v>
@@ -1159,7 +1277,14 @@
         <v>0.12986111111111112</v>
       </c>
       <c r="J22" t="n" s="10">
-        <v>51.0</v>
+        <v>51.5</v>
+      </c>
+      <c r="K22" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L22"/>
+      <c r="M22" t="n" s="12">
+        <v>1.0118055555555556</v>
       </c>
       <c r="O22" t="n" s="12">
         <v>0.89375</v>
@@ -1197,7 +1322,14 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="J23" t="n" s="10">
-        <v>22.0</v>
+        <v>22.5</v>
+      </c>
+      <c r="K23" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L23"/>
+      <c r="M23" t="n" s="12">
+        <v>0.9861111111111112</v>
       </c>
       <c r="O23" t="n" s="12">
         <v>0.875</v>
@@ -1235,7 +1367,14 @@
         <v>0.09027777777777778</v>
       </c>
       <c r="J24" t="n" s="10">
-        <v>59.0</v>
+        <v>59.5</v>
+      </c>
+      <c r="K24" t="n" s="12">
+        <v>0.3013888888888889</v>
+      </c>
+      <c r="L24"/>
+      <c r="M24" t="n" s="12">
+        <v>0.9909722222222223</v>
       </c>
       <c r="O24" t="n" s="12">
         <v>0.9152777777777777</v>
@@ -1275,6 +1414,13 @@
       <c r="J25" t="n" s="10">
         <v>54.0</v>
       </c>
+      <c r="K25" t="n" s="12">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="L25"/>
+      <c r="M25" t="n" s="12">
+        <v>0.9986111111111111</v>
+      </c>
       <c r="O25" t="n" s="12">
         <v>0.9097222222222222</v>
       </c>
@@ -1313,6 +1459,13 @@
       <c r="J26" t="n" s="10">
         <v>69.0</v>
       </c>
+      <c r="K26" t="n" s="12">
+        <v>0.2743055555555556</v>
+      </c>
+      <c r="L26"/>
+      <c r="M26" t="n" s="12">
+        <v>0.9784722222222222</v>
+      </c>
       <c r="O26" t="n" s="12">
         <v>0.9243055555555556</v>
       </c>
@@ -1349,7 +1502,14 @@
         <v>0.04861111111111111</v>
       </c>
       <c r="J27" t="n" s="10">
-        <v>11.0</v>
+        <v>11.5</v>
+      </c>
+      <c r="K27" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L27"/>
+      <c r="M27" t="n" s="12">
+        <v>0.9131944444444444</v>
       </c>
       <c r="O27" t="n" s="12">
         <v>0.8402777777777778</v>
@@ -1389,6 +1549,13 @@
       <c r="J28" t="n" s="10">
         <v>60.0</v>
       </c>
+      <c r="K28" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L28"/>
+      <c r="M28" t="n" s="12">
+        <v>0.9763888888888889</v>
+      </c>
       <c r="O28" t="n" s="12">
         <v>0.9256944444444445</v>
       </c>
@@ -1425,7 +1592,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J29" t="n" s="10">
-        <v>59.0</v>
+        <v>59.5</v>
+      </c>
+      <c r="K29" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L29"/>
+      <c r="M29" t="n" s="12">
+        <v>0.96875</v>
       </c>
       <c r="O29" t="n" s="12">
         <v>0.9270833333333334</v>
@@ -1463,7 +1637,14 @@
         <v>0.06875</v>
       </c>
       <c r="J30" t="n" s="10">
-        <v>27.0</v>
+        <v>27.5</v>
+      </c>
+      <c r="K30" t="n" s="12">
+        <v>0.29375</v>
+      </c>
+      <c r="L30"/>
+      <c r="M30" t="n" s="12">
+        <v>0.9791666666666666</v>
       </c>
       <c r="O30" t="n" s="12">
         <v>0.8986111111111111</v>
@@ -1501,7 +1682,14 @@
         <v>0.0625</v>
       </c>
       <c r="J31" t="n" s="10">
-        <v>29.0</v>
+        <v>29.5</v>
+      </c>
+      <c r="K31" t="n" s="12">
+        <v>0.28125</v>
+      </c>
+      <c r="L31"/>
+      <c r="M31" t="n" s="12">
+        <v>0.9756944444444444</v>
       </c>
       <c r="O31" t="n" s="12">
         <v>0.90625</v>
@@ -1539,7 +1727,14 @@
         <v>0.06944444444444445</v>
       </c>
       <c r="J32" t="n" s="10">
-        <v>43.0</v>
+        <v>43.5</v>
+      </c>
+      <c r="K32" t="n" s="12">
+        <v>0.28888888888888886</v>
+      </c>
+      <c r="L32"/>
+      <c r="M32" t="n" s="12">
+        <v>0.9833333333333333</v>
       </c>
       <c r="O32" t="n" s="12">
         <v>0.9138888888888889</v>
@@ -1577,7 +1772,14 @@
         <v>0.0625</v>
       </c>
       <c r="J33" t="n" s="10">
-        <v>42.0</v>
+        <v>42.5</v>
+      </c>
+      <c r="K33" t="n" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="L33"/>
+      <c r="M33" t="n" s="12">
+        <v>0.96875</v>
       </c>
       <c r="O33" t="n" s="12">
         <v>0.9215277777777777</v>
@@ -1615,7 +1817,14 @@
         <v>0.1</v>
       </c>
       <c r="J34" t="n" s="10">
-        <v>53.0</v>
+        <v>53.5</v>
+      </c>
+      <c r="K34" t="n" s="12">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="L34"/>
+      <c r="M34" t="n" s="12">
+        <v>0.9951388888888889</v>
       </c>
       <c r="O34" t="n" s="12">
         <v>0.8951388888888889</v>
@@ -1653,7 +1862,14 @@
         <v>0.09097222222222222</v>
       </c>
       <c r="J35" t="n" s="10">
-        <v>63.0</v>
+        <v>63.5</v>
+      </c>
+      <c r="K35" t="n" s="12">
+        <v>0.2673611111111111</v>
+      </c>
+      <c r="L35"/>
+      <c r="M35" t="n" s="12">
+        <v>0.9923611111111111</v>
       </c>
       <c r="O35" t="n" s="12">
         <v>0.9215277777777777</v>
@@ -1693,6 +1909,13 @@
       <c r="J36" t="n" s="10">
         <v>15.0</v>
       </c>
+      <c r="K36" t="n" s="12">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="L36"/>
+      <c r="M36" t="n" s="12">
+        <v>0.9375</v>
+      </c>
       <c r="O36" t="n" s="12">
         <v>0.8541666666666666</v>
       </c>
@@ -1729,7 +1952,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J37" t="n" s="10">
-        <v>87.0</v>
+        <v>87.5</v>
+      </c>
+      <c r="K37" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L37"/>
+      <c r="M37" t="n" s="12">
+        <v>0.9583333333333334</v>
       </c>
       <c r="O37" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -1769,6 +1999,13 @@
       <c r="J38" t="n" s="10">
         <v>63.0</v>
       </c>
+      <c r="K38" t="n" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="L38"/>
+      <c r="M38" t="n" s="12">
+        <v>1.0</v>
+      </c>
       <c r="O38" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
@@ -1807,6 +2044,13 @@
       <c r="J39" t="n" s="10">
         <v>105.0</v>
       </c>
+      <c r="K39" t="n" s="12">
+        <v>0.3194444444444444</v>
+      </c>
+      <c r="L39"/>
+      <c r="M39" t="n" s="12">
+        <v>0.975</v>
+      </c>
       <c r="O39" t="n" s="12">
         <v>0.925</v>
       </c>
@@ -1845,6 +2089,13 @@
       <c r="J40" t="n" s="10">
         <v>90.0</v>
       </c>
+      <c r="K40" t="n" s="12">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="L40"/>
+      <c r="M40" t="n" s="12">
+        <v>0.9729166666666667</v>
+      </c>
       <c r="O40" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
@@ -1881,7 +2132,14 @@
         <v>0.06041666666666667</v>
       </c>
       <c r="J41" t="n" s="10">
-        <v>30.0</v>
+        <v>30.5</v>
+      </c>
+      <c r="K41" t="n" s="12">
+        <v>0.3055555555555556</v>
+      </c>
+      <c r="L41"/>
+      <c r="M41" t="n" s="12">
+        <v>0.9722222222222222</v>
       </c>
       <c r="O41" t="n" s="12">
         <v>0.9097222222222222</v>
@@ -1921,6 +2179,13 @@
       <c r="J42" t="n" s="10">
         <v>23.0</v>
       </c>
+      <c r="K42" t="n" s="12">
+        <v>0.3055555555555556</v>
+      </c>
+      <c r="L42"/>
+      <c r="M42" t="n" s="12">
+        <v>0.9930555555555556</v>
+      </c>
       <c r="O42" t="n" s="12">
         <v>0.9097222222222222</v>
       </c>
@@ -1957,7 +2222,14 @@
         <v>0.05138888888888889</v>
       </c>
       <c r="J43" t="n" s="10">
-        <v>48.0</v>
+        <v>48.5</v>
+      </c>
+      <c r="K43" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L43"/>
+      <c r="M43" t="n" s="12">
+        <v>0.9729166666666667</v>
       </c>
       <c r="O43" t="n" s="12">
         <v>0.9208333333333333</v>
@@ -1997,6 +2269,13 @@
       <c r="J44" t="n" s="10">
         <v>42.0</v>
       </c>
+      <c r="K44" t="n" s="12">
+        <v>0.3020833333333333</v>
+      </c>
+      <c r="L44"/>
+      <c r="M44" t="n" s="12">
+        <v>0.96875</v>
+      </c>
       <c r="O44" t="n" s="12">
         <v>0.8854166666666666</v>
       </c>
@@ -2033,7 +2312,14 @@
         <v>0.03125</v>
       </c>
       <c r="J45" t="n" s="10">
-        <v>39.0</v>
+        <v>39.5</v>
+      </c>
+      <c r="K45" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L45"/>
+      <c r="M45" t="n" s="12">
+        <v>0.9527777777777777</v>
       </c>
       <c r="O45" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -2071,7 +2357,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J46" t="n" s="10">
-        <v>14.0</v>
+        <v>14.5</v>
+      </c>
+      <c r="K46" t="n" s="12">
+        <v>0.3194444444444444</v>
+      </c>
+      <c r="L46"/>
+      <c r="M46" t="n" s="12">
+        <v>0.9652777777777778</v>
       </c>
       <c r="O46" t="n" s="12">
         <v>0.9027777777777778</v>
@@ -2109,7 +2402,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J47" t="n" s="10">
-        <v>29.0</v>
+        <v>29.5</v>
+      </c>
+      <c r="K47" t="n" s="12">
+        <v>0.3055555555555556</v>
+      </c>
+      <c r="L47"/>
+      <c r="M47" t="n" s="12">
+        <v>0.9722222222222222</v>
       </c>
       <c r="O47" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -2149,6 +2449,13 @@
       <c r="J48" t="n" s="10">
         <v>54.0</v>
       </c>
+      <c r="K48" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L48"/>
+      <c r="M48" t="n" s="12">
+        <v>0.9916666666666667</v>
+      </c>
       <c r="O48" t="n" s="12">
         <v>0.9027777777777778</v>
       </c>
@@ -2185,7 +2492,14 @@
         <v>0.06944444444444445</v>
       </c>
       <c r="J49" t="n" s="10">
-        <v>34.0</v>
+        <v>34.5</v>
+      </c>
+      <c r="K49" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L49"/>
+      <c r="M49" t="n" s="12">
+        <v>0.9722222222222222</v>
       </c>
       <c r="O49" t="n" s="12">
         <v>0.9027777777777778</v>
@@ -2223,7 +2537,14 @@
         <v>0.06458333333333334</v>
       </c>
       <c r="J50" t="n" s="10">
-        <v>55.0</v>
+        <v>55.5</v>
+      </c>
+      <c r="K50" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L50"/>
+      <c r="M50" t="n" s="12">
+        <v>0.9805555555555555</v>
       </c>
       <c r="O50" t="n" s="12">
         <v>0.9263888888888889</v>
@@ -2263,6 +2584,13 @@
       <c r="J51" t="n" s="10">
         <v>59.0</v>
       </c>
+      <c r="K51" t="n" s="12">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="L51"/>
+      <c r="M51" t="n" s="12">
+        <v>0.9861111111111112</v>
+      </c>
       <c r="O51" t="n" s="12">
         <v>0.9236111111111112</v>
       </c>
@@ -2299,7 +2627,14 @@
         <v>0.13541666666666666</v>
       </c>
       <c r="J52" t="n" s="10">
-        <v>59.0</v>
+        <v>59.5</v>
+      </c>
+      <c r="K52" t="n" s="12">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="L52"/>
+      <c r="M52" t="n" s="12">
+        <v>1.0104166666666667</v>
       </c>
       <c r="O52" t="n" s="12">
         <v>0.8854166666666666</v>
@@ -2337,7 +2672,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J53" t="n" s="10">
-        <v>43.0</v>
+        <v>43.5</v>
+      </c>
+      <c r="K53" t="n" s="12">
+        <v>0.3020833333333333</v>
+      </c>
+      <c r="L53"/>
+      <c r="M53" t="n" s="12">
+        <v>0.96875</v>
       </c>
       <c r="O53" t="n" s="12">
         <v>0.9270833333333334</v>
@@ -2377,6 +2719,13 @@
       <c r="J54" t="n" s="10">
         <v>37.0</v>
       </c>
+      <c r="K54" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L54"/>
+      <c r="M54" t="n" s="12">
+        <v>0.9756944444444444</v>
+      </c>
       <c r="O54" t="n" s="12">
         <v>0.9194444444444444</v>
       </c>
@@ -2413,7 +2762,14 @@
         <v>0.09583333333333334</v>
       </c>
       <c r="J55" t="n" s="10">
-        <v>37.0</v>
+        <v>37.5</v>
+      </c>
+      <c r="K55" t="n" s="12">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="L55"/>
+      <c r="M55" t="n" s="12">
+        <v>0.9979166666666667</v>
       </c>
       <c r="O55" t="n" s="12">
         <v>0.9020833333333333</v>
@@ -2451,7 +2807,14 @@
         <v>0.0625</v>
       </c>
       <c r="J56" t="n" s="10">
-        <v>49.0</v>
+        <v>49.5</v>
+      </c>
+      <c r="K56" t="n" s="12">
+        <v>0.3055555555555556</v>
+      </c>
+      <c r="L56"/>
+      <c r="M56" t="n" s="12">
+        <v>0.9805555555555555</v>
       </c>
       <c r="O56" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -2489,7 +2852,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J57" t="n" s="10">
-        <v>14.0</v>
+        <v>14.5</v>
+      </c>
+      <c r="K57" t="n" s="12">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="L57"/>
+      <c r="M57" t="n" s="12">
+        <v>0.9756944444444444</v>
       </c>
       <c r="O57" t="n" s="12">
         <v>0.9131944444444444</v>
@@ -2527,7 +2897,14 @@
         <v>0.06944444444444445</v>
       </c>
       <c r="J58" t="n" s="10">
-        <v>32.0</v>
+        <v>32.5</v>
+      </c>
+      <c r="K58" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L58"/>
+      <c r="M58" t="n" s="12">
+        <v>0.9722222222222222</v>
       </c>
       <c r="O58" t="n" s="12">
         <v>0.9027777777777778</v>
@@ -2567,6 +2944,13 @@
       <c r="J59" t="n" s="10">
         <v>61.0</v>
       </c>
+      <c r="K59" t="n" s="12">
+        <v>0.3020833333333333</v>
+      </c>
+      <c r="L59"/>
+      <c r="M59" t="n" s="12">
+        <v>0.9784722222222222</v>
+      </c>
       <c r="O59" t="n" s="12">
         <v>0.9243055555555556</v>
       </c>
@@ -2605,6 +2989,13 @@
       <c r="J60" t="n" s="10">
         <v>51.0</v>
       </c>
+      <c r="K60" t="n" s="12">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="L60"/>
+      <c r="M60" t="n" s="12">
+        <v>0.9833333333333333</v>
+      </c>
       <c r="O60" t="n" s="12">
         <v>0.9083333333333333</v>
       </c>
@@ -2643,6 +3034,13 @@
       <c r="J61" t="n" s="10">
         <v>52.0</v>
       </c>
+      <c r="K61" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L61"/>
+      <c r="M61" t="n" s="12">
+        <v>0.9881944444444445</v>
+      </c>
       <c r="O61" t="n" s="12">
         <v>0.9055555555555556</v>
       </c>
@@ -2679,7 +3077,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J62" t="n" s="10">
-        <v>14.0</v>
+        <v>14.5</v>
+      </c>
+      <c r="K62" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L62"/>
+      <c r="M62" t="n" s="12">
+        <v>0.9583333333333334</v>
       </c>
       <c r="O62" t="n" s="12">
         <v>0.8958333333333334</v>
@@ -2717,7 +3122,14 @@
         <v>0.03333333333333333</v>
       </c>
       <c r="J63" t="n" s="10">
-        <v>35.0</v>
+        <v>35.5</v>
+      </c>
+      <c r="K63" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L63"/>
+      <c r="M63" t="n" s="12">
+        <v>0.9458333333333333</v>
       </c>
       <c r="O63" t="n" s="12">
         <v>0.9125</v>
@@ -2755,7 +3167,14 @@
         <v>0.03125</v>
       </c>
       <c r="J64" t="n" s="10">
-        <v>18.0</v>
+        <v>18.5</v>
+      </c>
+      <c r="K64" t="n" s="12">
+        <v>0.3229166666666667</v>
+      </c>
+      <c r="L64"/>
+      <c r="M64" t="n" s="12">
+        <v>0.9326388888888889</v>
       </c>
       <c r="O64" t="n" s="12">
         <v>0.8854166666666666</v>
@@ -2795,6 +3214,13 @@
       <c r="J65" t="n" s="10">
         <v>50.0</v>
       </c>
+      <c r="K65" t="n" s="12">
+        <v>0.3194444444444444</v>
+      </c>
+      <c r="L65"/>
+      <c r="M65" t="n" s="12">
+        <v>0.9625</v>
+      </c>
       <c r="O65" t="n" s="12">
         <v>0.9215277777777777</v>
       </c>
@@ -2833,6 +3259,13 @@
       <c r="J66" t="n" s="10">
         <v>51.0</v>
       </c>
+      <c r="K66" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L66"/>
+      <c r="M66" t="n" s="12">
+        <v>0.9868055555555556</v>
+      </c>
       <c r="O66" t="n" s="12">
         <v>0.9236111111111112</v>
       </c>
@@ -2871,6 +3304,13 @@
       <c r="J67" t="n" s="10">
         <v>61.0</v>
       </c>
+      <c r="K67" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L67"/>
+      <c r="M67" t="n" s="12">
+        <v>0.9881944444444445</v>
+      </c>
       <c r="O67" t="n" s="12">
         <v>0.9138888888888889</v>
       </c>
@@ -2907,7 +3347,14 @@
         <v>0.06458333333333334</v>
       </c>
       <c r="J68" t="n" s="10">
-        <v>60.0</v>
+        <v>60.5</v>
+      </c>
+      <c r="K68" t="n" s="12">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="L68"/>
+      <c r="M68" t="n" s="12">
+        <v>0.9708333333333333</v>
       </c>
       <c r="O68" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -2945,7 +3392,14 @@
         <v>0.029166666666666667</v>
       </c>
       <c r="J69" t="n" s="10">
-        <v>65.0</v>
+        <v>65.5</v>
+      </c>
+      <c r="K69" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L69"/>
+      <c r="M69" t="n" s="12">
+        <v>0.9625</v>
       </c>
       <c r="O69" t="n" s="12">
         <v>0.9333333333333333</v>
@@ -2985,6 +3439,13 @@
       <c r="J70" t="n" s="10">
         <v>15.0</v>
       </c>
+      <c r="K70" t="n" s="12">
+        <v>0.2708333333333333</v>
+      </c>
+      <c r="L70"/>
+      <c r="M70" t="n" s="12">
+        <v>0.9375</v>
+      </c>
       <c r="O70" t="n" s="12">
         <v>0.8541666666666666</v>
       </c>
@@ -3021,7 +3482,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J71" t="n" s="10">
-        <v>31.0</v>
+        <v>31.5</v>
+      </c>
+      <c r="K71" t="n" s="12">
+        <v>0.2847222222222222</v>
+      </c>
+      <c r="L71"/>
+      <c r="M71" t="n" s="12">
+        <v>0.9722222222222222</v>
       </c>
       <c r="O71" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -3059,7 +3527,14 @@
         <v>0.034722222222222224</v>
       </c>
       <c r="J72" t="n" s="10">
-        <v>18.0</v>
+        <v>18.5</v>
+      </c>
+      <c r="K72" t="n" s="12">
+        <v>0.2881944444444444</v>
+      </c>
+      <c r="L72"/>
+      <c r="M72" t="n" s="12">
+        <v>0.9618055555555556</v>
       </c>
       <c r="O72" t="n" s="12">
         <v>0.9097222222222222</v>
@@ -3099,6 +3574,13 @@
       <c r="J73" t="n" s="10">
         <v>55.0</v>
       </c>
+      <c r="K73" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L73"/>
+      <c r="M73" t="n" s="12">
+        <v>0.9583333333333334</v>
+      </c>
       <c r="O73" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
@@ -3135,7 +3617,14 @@
         <v>0.022222222222222223</v>
       </c>
       <c r="J74" t="n" s="10">
-        <v>57.0</v>
+        <v>57.5</v>
+      </c>
+      <c r="K74" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L74"/>
+      <c r="M74" t="n" s="12">
+        <v>0.9583333333333334</v>
       </c>
       <c r="O74" t="n" s="12">
         <v>0.9361111111111111</v>
@@ -3173,7 +3662,14 @@
         <v>0.04861111111111111</v>
       </c>
       <c r="J75" t="n" s="10">
-        <v>12.0</v>
+        <v>12.5</v>
+      </c>
+      <c r="K75" t="n" s="12">
+        <v>0.3090277777777778</v>
+      </c>
+      <c r="L75"/>
+      <c r="M75" t="n" s="12">
+        <v>0.9604166666666667</v>
       </c>
       <c r="O75" t="n" s="12">
         <v>0.8854166666666666</v>
@@ -3211,7 +3707,14 @@
         <v>0.0625</v>
       </c>
       <c r="J76" t="n" s="10">
-        <v>8.0</v>
+        <v>8.5</v>
+      </c>
+      <c r="K76" t="n" s="12">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="L76"/>
+      <c r="M76" t="n" s="12">
+        <v>0.9055555555555556</v>
       </c>
       <c r="O76" t="n" s="12">
         <v>0.8118055555555556</v>
@@ -3251,6 +3754,13 @@
       <c r="J77" t="n" s="10">
         <v>13.0</v>
       </c>
+      <c r="K77" t="n" s="12">
+        <v>0.3020833333333333</v>
+      </c>
+      <c r="L77"/>
+      <c r="M77" t="n" s="12">
+        <v>0.9270833333333334</v>
+      </c>
       <c r="O77" t="n" s="12">
         <v>0.84375</v>
       </c>
@@ -3287,7 +3797,14 @@
         <v>0.075</v>
       </c>
       <c r="J78" t="n" s="10">
-        <v>32.0</v>
+        <v>32.5</v>
+      </c>
+      <c r="K78" t="n" s="12">
+        <v>0.30416666666666664</v>
+      </c>
+      <c r="L78"/>
+      <c r="M78" t="n" s="12">
+        <v>0.9840277777777777</v>
       </c>
       <c r="O78" t="n" s="12">
         <v>0.9041666666666667</v>
@@ -3327,6 +3844,13 @@
       <c r="J79" t="n" s="10">
         <v>52.0</v>
       </c>
+      <c r="K79" t="n" s="12">
+        <v>0.2951388888888889</v>
+      </c>
+      <c r="L79"/>
+      <c r="M79" t="n" s="12">
+        <v>0.9840277777777777</v>
+      </c>
       <c r="O79" t="n" s="12">
         <v>0.8951388888888889</v>
       </c>
@@ -3365,6 +3889,13 @@
       <c r="J80" t="n" s="10">
         <v>43.0</v>
       </c>
+      <c r="K80" t="n" s="12">
+        <v>0.29583333333333334</v>
+      </c>
+      <c r="L80"/>
+      <c r="M80" t="n" s="12">
+        <v>0.98125</v>
+      </c>
       <c r="O80" t="n" s="12">
         <v>0.9083333333333333</v>
       </c>
@@ -3403,6 +3934,13 @@
       <c r="J81" t="n" s="10">
         <v>71.0</v>
       </c>
+      <c r="K81" t="n" s="12">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="L81"/>
+      <c r="M81" t="n" s="12">
+        <v>0.9805555555555555</v>
+      </c>
       <c r="O81" t="n" s="12">
         <v>0.9111111111111111</v>
       </c>
@@ -3439,7 +3977,14 @@
         <v>0.04583333333333333</v>
       </c>
       <c r="J82" t="n" s="10">
-        <v>26.0</v>
+        <v>26.5</v>
+      </c>
+      <c r="K82" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L82"/>
+      <c r="M82" t="n" s="12">
+        <v>0.9583333333333334</v>
       </c>
       <c r="O82" t="n" s="12">
         <v>0.9090277777777778</v>
@@ -3479,6 +4024,13 @@
       <c r="J83" t="n" s="10">
         <v>58.0</v>
       </c>
+      <c r="K83" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L83"/>
+      <c r="M83" t="n" s="12">
+        <v>0.9729166666666667</v>
+      </c>
       <c r="O83" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
@@ -3517,6 +4069,13 @@
       <c r="J84" t="n" s="10">
         <v>33.0</v>
       </c>
+      <c r="K84" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L84"/>
+      <c r="M84" t="n" s="12">
+        <v>0.9666666666666667</v>
+      </c>
       <c r="O84" t="n" s="12">
         <v>0.9020833333333333</v>
       </c>
@@ -3553,7 +4112,14 @@
         <v>0.0625</v>
       </c>
       <c r="J85" t="n" s="10">
-        <v>49.0</v>
+        <v>49.5</v>
+      </c>
+      <c r="K85" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L85"/>
+      <c r="M85" t="n" s="12">
+        <v>0.9791666666666666</v>
       </c>
       <c r="O85" t="n" s="12">
         <v>0.9166666666666666</v>
@@ -3591,7 +4157,14 @@
         <v>0.04722222222222222</v>
       </c>
       <c r="J86" t="n" s="10">
-        <v>51.0</v>
+        <v>51.5</v>
+      </c>
+      <c r="K86" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L86"/>
+      <c r="M86" t="n" s="12">
+        <v>0.9645833333333333</v>
       </c>
       <c r="O86" t="n" s="12">
         <v>0.9173611111111111</v>
@@ -3629,7 +4202,14 @@
         <v>0.09930555555555555</v>
       </c>
       <c r="J87" t="n" s="10">
-        <v>40.0</v>
+        <v>40.5</v>
+      </c>
+      <c r="K87" t="n" s="12">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="L87"/>
+      <c r="M87" t="n" s="12">
+        <v>0.9958333333333333</v>
       </c>
       <c r="O87" t="n" s="12">
         <v>0.8965277777777778</v>
@@ -3667,7 +4247,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J88" t="n" s="10">
-        <v>57.0</v>
+        <v>57.5</v>
+      </c>
+      <c r="K88" t="n" s="12">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="L88"/>
+      <c r="M88" t="n" s="12">
+        <v>0.9652777777777778</v>
       </c>
       <c r="O88" t="n" s="12">
         <v>0.9236111111111112</v>
@@ -3707,6 +4294,13 @@
       <c r="J89" t="n" s="10">
         <v>33.0</v>
       </c>
+      <c r="K89" t="n" s="12">
+        <v>0.2972222222222222</v>
+      </c>
+      <c r="L89"/>
+      <c r="M89" t="n" s="12">
+        <v>1.0006944444444446</v>
+      </c>
       <c r="O89" t="n" s="12">
         <v>0.9159722222222222</v>
       </c>
@@ -3745,6 +4339,13 @@
       <c r="J90" t="n" s="10">
         <v>34.0</v>
       </c>
+      <c r="K90" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L90"/>
+      <c r="M90" t="n" s="12">
+        <v>0.9958333333333333</v>
+      </c>
       <c r="O90" t="n" s="12">
         <v>0.9055555555555556</v>
       </c>
@@ -3781,7 +4382,14 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="J91" t="n" s="10">
-        <v>22.0</v>
+        <v>22.5</v>
+      </c>
+      <c r="K91" t="n" s="12">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="L91"/>
+      <c r="M91" t="n" s="12">
+        <v>0.9701388888888889</v>
       </c>
       <c r="O91" t="n" s="12">
         <v>0.9020833333333333</v>
@@ -3821,6 +4429,13 @@
       <c r="J92" t="n" s="10">
         <v>25.0</v>
       </c>
+      <c r="K92" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L92"/>
+      <c r="M92" t="n" s="12">
+        <v>0.9479166666666666</v>
+      </c>
       <c r="O92" t="n" s="12">
         <v>0.8993055555555556</v>
       </c>
@@ -3857,7 +4472,14 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="J93" t="n" s="10">
-        <v>22.0</v>
+        <v>22.5</v>
+      </c>
+      <c r="K93" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L93"/>
+      <c r="M93" t="n" s="12">
+        <v>0.9861111111111112</v>
       </c>
       <c r="O93" t="n" s="12">
         <v>0.8756944444444444</v>
@@ -3895,7 +4517,14 @@
         <v>0.0763888888888889</v>
       </c>
       <c r="J94" t="n" s="10">
-        <v>8.0</v>
+        <v>8.5</v>
+      </c>
+      <c r="K94" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L94"/>
+      <c r="M94" t="n" s="12">
+        <v>0.9826388888888888</v>
       </c>
       <c r="O94" t="n" s="12">
         <v>0.8680555555555556</v>
@@ -3935,6 +4564,13 @@
       <c r="J95" t="n" s="10">
         <v>36.0</v>
       </c>
+      <c r="K95" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L95"/>
+      <c r="M95" t="n" s="12">
+        <v>0.9861111111111112</v>
+      </c>
       <c r="O95" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
@@ -3971,7 +4607,14 @@
         <v>0.04861111111111111</v>
       </c>
       <c r="J96" t="n" s="10">
-        <v>12.0</v>
+        <v>12.5</v>
+      </c>
+      <c r="K96" t="n" s="12">
+        <v>0.3194444444444444</v>
+      </c>
+      <c r="L96"/>
+      <c r="M96" t="n" s="12">
+        <v>0.9666666666666667</v>
       </c>
       <c r="O96" t="n" s="12">
         <v>0.8958333333333334</v>
@@ -4011,6 +4654,13 @@
       <c r="J97" t="n" s="10">
         <v>30.0</v>
       </c>
+      <c r="K97" t="n" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="L97"/>
+      <c r="M97" t="n" s="12">
+        <v>0.9583333333333334</v>
+      </c>
       <c r="O97" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
@@ -4047,7 +4697,14 @@
         <v>0.08333333333333333</v>
       </c>
       <c r="J98" t="n" s="10">
-        <v>21.0</v>
+        <v>21.5</v>
+      </c>
+      <c r="K98" t="n" s="12">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="L98"/>
+      <c r="M98" t="n" s="12">
+        <v>0.9631944444444445</v>
       </c>
       <c r="O98" t="n" s="12">
         <v>0.89375</v>
@@ -4087,6 +4744,13 @@
       <c r="J99" t="n" s="10">
         <v>56.0</v>
       </c>
+      <c r="K99" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L99"/>
+      <c r="M99" t="n" s="12">
+        <v>0.9756944444444444</v>
+      </c>
       <c r="O99" t="n" s="12">
         <v>0.925</v>
       </c>
@@ -4123,7 +4787,14 @@
         <v>0.04861111111111111</v>
       </c>
       <c r="J100" t="n" s="10">
-        <v>25.0</v>
+        <v>25.5</v>
+      </c>
+      <c r="K100" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L100"/>
+      <c r="M100" t="n" s="12">
+        <v>0.9479166666666666</v>
       </c>
       <c r="O100" t="n" s="12">
         <v>0.8993055555555556</v>
@@ -4163,6 +4834,13 @@
       <c r="J101" t="n" s="10">
         <v>36.0</v>
       </c>
+      <c r="K101" t="n" s="12">
+        <v>0.3541666666666667</v>
+      </c>
+      <c r="L101"/>
+      <c r="M101" t="n" s="12">
+        <v>0.9770833333333333</v>
+      </c>
       <c r="O101" t="n" s="12">
         <v>0.9131944444444444</v>
       </c>
@@ -4201,6 +4879,13 @@
       <c r="J102" t="n" s="10">
         <v>82.0</v>
       </c>
+      <c r="K102" t="n" s="12">
+        <v>0.2881944444444444</v>
+      </c>
+      <c r="L102"/>
+      <c r="M102" t="n" s="12">
+        <v>0.9826388888888888</v>
+      </c>
       <c r="O102" t="n" s="12">
         <v>0.9375</v>
       </c>
@@ -4237,7 +4922,14 @@
         <v>0.13333333333333333</v>
       </c>
       <c r="J103" t="n" s="10">
-        <v>75.0</v>
+        <v>75.5</v>
+      </c>
+      <c r="K103" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L103"/>
+      <c r="M103" t="n" s="12">
+        <v>1.011111111111111</v>
       </c>
       <c r="O103" t="n" s="12">
         <v>0.9354166666666667</v>
@@ -4275,7 +4967,14 @@
         <v>0.041666666666666664</v>
       </c>
       <c r="J104" t="n" s="10">
-        <v>59.0</v>
+        <v>59.5</v>
+      </c>
+      <c r="K104" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L104"/>
+      <c r="M104" t="n" s="12">
+        <v>0.9652777777777778</v>
       </c>
       <c r="O104" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -4315,6 +5014,13 @@
       <c r="J105" t="n" s="10">
         <v>60.0</v>
       </c>
+      <c r="K105" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L105"/>
+      <c r="M105" t="n" s="12">
+        <v>0.9861111111111112</v>
+      </c>
       <c r="O105" t="n" s="12">
         <v>0.9305555555555556</v>
       </c>
@@ -4353,6 +5059,13 @@
       <c r="J106" t="n" s="10">
         <v>69.0</v>
       </c>
+      <c r="K106" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L106"/>
+      <c r="M106" t="n" s="12">
+        <v>0.9729166666666667</v>
+      </c>
       <c r="O106" t="n" s="12">
         <v>0.9256944444444445</v>
       </c>
@@ -4391,6 +5104,13 @@
       <c r="J107" t="n" s="10">
         <v>136.0</v>
       </c>
+      <c r="K107" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L107"/>
+      <c r="M107" t="n" s="12">
+        <v>0.9673611111111111</v>
+      </c>
       <c r="O107" t="n" s="12">
         <v>0.9430555555555555</v>
       </c>
@@ -4427,7 +5147,14 @@
         <v>0.09375</v>
       </c>
       <c r="J108" t="n" s="10">
-        <v>61.0</v>
+        <v>61.5</v>
+      </c>
+      <c r="K108" t="n" s="12">
+        <v>0.2881944444444444</v>
+      </c>
+      <c r="L108"/>
+      <c r="M108" t="n" s="12">
+        <v>0.9916666666666667</v>
       </c>
       <c r="O108" t="n" s="12">
         <v>0.9291666666666667</v>
@@ -4467,6 +5194,13 @@
       <c r="J109" t="n" s="10">
         <v>92.0</v>
       </c>
+      <c r="K109" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L109"/>
+      <c r="M109" t="n" s="12">
+        <v>0.9722222222222222</v>
+      </c>
       <c r="O109" t="n" s="12">
         <v>0.9347222222222222</v>
       </c>
@@ -4503,7 +5237,14 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="J110" t="n" s="10">
-        <v>89.0</v>
+        <v>89.5</v>
+      </c>
+      <c r="K110" t="n" s="12">
+        <v>0.2881944444444444</v>
+      </c>
+      <c r="L110"/>
+      <c r="M110" t="n" s="12">
+        <v>0.9930555555555556</v>
       </c>
       <c r="O110" t="n" s="12">
         <v>0.9305555555555556</v>
@@ -4543,6 +5284,13 @@
       <c r="J111" t="n" s="10">
         <v>71.0</v>
       </c>
+      <c r="K111" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L111"/>
+      <c r="M111" t="n" s="12">
+        <v>0.9868055555555556</v>
+      </c>
       <c r="O111" t="n" s="12">
         <v>0.9326388888888889</v>
       </c>
@@ -4581,6 +5329,13 @@
       <c r="J112" t="n" s="10">
         <v>64.0</v>
       </c>
+      <c r="K112" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L112"/>
+      <c r="M112" t="n" s="12">
+        <v>0.9777777777777777</v>
+      </c>
       <c r="O112" t="n" s="12">
         <v>0.9263888888888889</v>
       </c>
@@ -4619,6 +5374,13 @@
       <c r="J113" t="n" s="10">
         <v>71.0</v>
       </c>
+      <c r="K113" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L113"/>
+      <c r="M113" t="n" s="12">
+        <v>0.9784722222222222</v>
+      </c>
       <c r="O113" t="n" s="12">
         <v>0.9333333333333333</v>
       </c>
@@ -4657,6 +5419,13 @@
       <c r="J114" t="n" s="10">
         <v>68.0</v>
       </c>
+      <c r="K114" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L114"/>
+      <c r="M114" t="n" s="12">
+        <v>0.9722222222222222</v>
+      </c>
       <c r="O114" t="n" s="12">
         <v>0.9333333333333333</v>
       </c>
@@ -4694,6 +5463,13 @@
       </c>
       <c r="J115" t="n" s="10">
         <v>84.0</v>
+      </c>
+      <c r="K115" t="n" s="12">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="L115"/>
+      <c r="M115" t="n" s="12">
+        <v>0.9701388888888889</v>
       </c>
       <c r="O115" t="n" s="12">
         <v>0.9298611111111111</v>

</xml_diff>